<commit_message>
- Updated parts list with alternate usb adapters
</commit_message>
<xml_diff>
--- a/SecureSyncStations/OPE Sync Station - Parts List.xlsx
+++ b/SecureSyncStations/OPE Sync Station - Parts List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Part</t>
   </si>
@@ -211,6 +211,21 @@
   <si>
     <t>NEED USB 3.0 for full speed, don't go below USB 2.0</t>
   </si>
+  <si>
+    <t>https://www.amazon.com/Dell-FM76N-ETHERNET-DBJBCBC064-Optiplex/dp/B00UK8N0TK/ref=sr_1_1?dchild=1&amp;keywords=DBJBCBC064&amp;qid=1587588576&amp;sr=8-1</t>
+  </si>
+  <si>
+    <t>Alternate USB to Nic Adaptor</t>
+  </si>
+  <si>
+    <t>Alternate Dell Model</t>
+  </si>
+  <si>
+    <t>Lenovo Model</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Lenovo-4X90E51405-Thinkpad-Ethernet-Compatible/dp/B00GKBL4NA/ref=sr_1_1?crid=1B8ZAXDILJZM3&amp;dchild=1&amp;keywords=lenovo+rtl8153&amp;qid=1591723697&amp;s=electronics&amp;sprefix=lenovo+rtl%2Celectronics%2C216&amp;sr=1-1</t>
+  </si>
 </sst>
 </file>
 
@@ -219,7 +234,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,6 +254,22 @@
       <b/>
       <sz val="11"/>
       <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -273,10 +304,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -286,8 +318,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -566,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,7 +677,7 @@
       <c r="E5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="9" t="s">
         <v>4</v>
       </c>
     </row>
@@ -956,8 +991,38 @@
         <v>500</v>
       </c>
     </row>
+    <row r="25" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A25" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A27" r:id="rId1"/>
+    <hyperlink ref="F5" r:id="rId2"/>
+    <hyperlink ref="A29" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Update USB Nic links and alt cat 5 keystone coupler.
</commit_message>
<xml_diff>
--- a/SecureSyncStations/OPE Sync Station - Parts List.xlsx
+++ b/SecureSyncStations/OPE Sync Station - Parts List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Part</t>
   </si>
@@ -225,6 +225,12 @@
   </si>
   <si>
     <t>https://www.amazon.com/Lenovo-4X90E51405-Thinkpad-Ethernet-Compatible/dp/B00GKBL4NA/ref=sr_1_1?crid=1B8ZAXDILJZM3&amp;dchild=1&amp;keywords=lenovo+rtl8153&amp;qid=1591723697&amp;s=electronics&amp;sprefix=lenovo+rtl%2Celectronics%2C216&amp;sr=1-1</t>
+  </si>
+  <si>
+    <t>Alternate Keystone Cat 5 Part</t>
+  </si>
+  <si>
+    <t>https://www.cdw.com/product/Black-Box-Keystone-network-coupler-black/1618009?cm_cat=google&amp;cm_ite=1618009&amp;cm_pla=NA-NA-Black%20Box_CN&amp;cm_ven=acquirgy&amp;ef_id=Cj0KCQjw0Mb3BRCaARIsAPSNGpUoX6X39ddO85-UXGQzn5N_tQEbaiegaa_2YFLvYHZzPBWxzRLsVKgaAi6TEALw_wcB:G:s&amp;gclid=Cj0KCQjw0Mb3BRCaARIsAPSNGpUoX6X39ddO85-UXGQzn5N_tQEbaiegaa_2YFLvYHZzPBWxzRLsVKgaAi6TEALw_wcB&amp;s_kwcid=AL!4223!3!324844189100!!!g!339799153589!</t>
   </si>
 </sst>
 </file>
@@ -601,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:A30"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,6 +1022,16 @@
         <v>58</v>
       </c>
     </row>
+    <row r="31" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A31" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A27" r:id="rId1"/>

</xml_diff>

<commit_message>
- Update link for t8 torx security bits
</commit_message>
<xml_diff>
--- a/SecureSyncStations/OPE Sync Station - Parts List.xlsx
+++ b/SecureSyncStations/OPE Sync Station - Parts List.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="Sync Box Parts List" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Part</t>
   </si>
@@ -232,11 +232,14 @@
   <si>
     <t>https://www.cdw.com/product/Black-Box-Keystone-network-coupler-black/1618009?cm_cat=google&amp;cm_ite=1618009&amp;cm_pla=NA-NA-Black%20Box_CN&amp;cm_ven=acquirgy&amp;ef_id=Cj0KCQjw0Mb3BRCaARIsAPSNGpUoX6X39ddO85-UXGQzn5N_tQEbaiegaa_2YFLvYHZzPBWxzRLsVKgaAi6TEALw_wcB:G:s&amp;gclid=Cj0KCQjw0Mb3BRCaARIsAPSNGpUoX6X39ddO85-UXGQzn5N_tQEbaiegaa_2YFLvYHZzPBWxzRLsVKgaAi6TEALw_wcB&amp;s_kwcid=AL!4223!3!324844189100!!!g!339799153589!</t>
   </si>
+  <si>
+    <t>https://www.amazon.com/Piece-Security-Torx-Bit-Set/dp/B07BKQ5237/ref=sr_1_5?crid=2HM9YJOQDT6LN&amp;keywords=t-8+torx+security&amp;qid=1640200603&amp;s=hi&amp;sprefix=t-8+torx+security%2Ctools%2C1192&amp;sr=1-5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
@@ -607,27 +610,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="39.44140625" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -647,7 +650,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -667,7 +670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -687,7 +690,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -707,7 +710,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -725,7 +728,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -743,7 +746,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -761,7 +764,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -781,7 +784,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -799,7 +802,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -817,7 +820,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -835,7 +838,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -853,7 +856,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -871,7 +874,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -886,7 +889,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>49</v>
       </c>
@@ -906,7 +909,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -926,7 +929,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -946,7 +949,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -963,10 +966,13 @@
         <v>38</v>
       </c>
       <c r="F20" t="s">
+        <v>61</v>
+      </c>
+      <c r="L20" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>39</v>
       </c>
@@ -983,13 +989,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D24" s="1" t="s">
         <v>47</v>
       </c>
@@ -997,37 +1003,37 @@
         <v>500</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:12" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A25" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:12" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A31" s="10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>60</v>
       </c>
@@ -1037,8 +1043,9 @@
     <hyperlink ref="A27" r:id="rId1"/>
     <hyperlink ref="F5" r:id="rId2"/>
     <hyperlink ref="A29" r:id="rId3"/>
+    <hyperlink ref="L20" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>